<commit_message>
Committing Revlon & Hot Tools Smoke System tests
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
+++ b/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B585D0AF-37C1-46BD-9F21-C804B5B899A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="5925"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
   <si>
     <t>UserName</t>
   </si>
@@ -28,9 +36,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>mahendr.selenium@gmail.com</t>
-  </si>
-  <si>
     <t>DataSet</t>
   </si>
   <si>
@@ -43,15 +48,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>mahendra</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>Mahendra123</t>
-  </si>
-  <si>
     <t>Street</t>
   </si>
   <si>
@@ -142,9 +138,6 @@
     <t>MiddleName</t>
   </si>
   <si>
-    <t>Kumar</t>
-  </si>
-  <si>
     <t>shippingAddress</t>
   </si>
   <si>
@@ -166,17 +159,131 @@
     <t>HOT TOOLS AMETHYST DRYER</t>
   </si>
   <si>
-    <t>yoga.manoj6@gmail.com</t>
+    <t>harish.chiruvella1@gmail.com</t>
+  </si>
+  <si>
+    <t>Harish!123</t>
+  </si>
+  <si>
+    <t>Harish</t>
+  </si>
+  <si>
+    <t>Chiruvella</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Addressbook</t>
+  </si>
+  <si>
+    <t>Lotuswave</t>
+  </si>
+  <si>
+    <t>ProductReview</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>Nice Product. The Hot Tools Amethyst Turbo Dryer is a lightweight, compact tool with all the power of a full-sized dryer, adorned in a chic, amethyst hue.</t>
+  </si>
+  <si>
+    <t>FEATURED PRODUCTS</t>
+  </si>
+  <si>
+    <t>homePage</t>
+  </si>
+  <si>
+    <t>HomePage</t>
+  </si>
+  <si>
+    <t>Retailer_registration</t>
+  </si>
+  <si>
+    <t>harish.chiruvella1988@gmail.com</t>
+  </si>
+  <si>
+    <t>Mini Travel Dryer in Mint</t>
+  </si>
+  <si>
+    <t>alonsogarcia+pro@gmail.com</t>
+  </si>
+  <si>
+    <t>Testpro123</t>
+  </si>
+  <si>
+    <t>DistributorAccountDetails</t>
+  </si>
+  <si>
+    <t>Stylist_registration</t>
+  </si>
+  <si>
+    <t>License Expiration Date</t>
+  </si>
+  <si>
+    <t>License Number</t>
+  </si>
+  <si>
+    <t>Upload License</t>
+  </si>
+  <si>
+    <t>Estimated Number</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>AFGHJKLKL</t>
+  </si>
+  <si>
+    <t>D:\test image.jpg</t>
+  </si>
+  <si>
+    <t>05/06/1989</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>State Associated</t>
+  </si>
+  <si>
+    <t>11/30/2020</t>
+  </si>
+  <si>
+    <t>ProductRegistration</t>
+  </si>
+  <si>
+    <t>Storewherepurchased</t>
+  </si>
+  <si>
+    <t>Customer Type</t>
+  </si>
+  <si>
+    <t>Salon Owner</t>
+  </si>
+  <si>
+    <t>Producttype</t>
+  </si>
+  <si>
+    <t>harish@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +295,26 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -220,13 +347,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -507,11 +646,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AO12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +660,7 @@
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
@@ -536,11 +676,23 @@
     <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="24" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="45.28515625" style="6" customWidth="1"/>
+    <col min="31" max="31" width="20.7109375" style="6" customWidth="1"/>
+    <col min="32" max="32" width="22" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="26" customWidth="1"/>
+    <col min="35" max="35" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.42578125" customWidth="1"/>
+    <col min="39" max="39" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -549,105 +701,147 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="M2">
         <v>12345</v>
       </c>
       <c r="V2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="W2">
         <v>1994</v>
@@ -655,100 +849,304 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="N3" s="4">
+        <v>58</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4">
+        <v>12345</v>
+      </c>
+      <c r="N4">
         <v>9898989899</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="X3" t="s">
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AF4" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ4">
+        <v>30</v>
+      </c>
+      <c r="AK4" s="4">
+        <v>9898989899</v>
+      </c>
+      <c r="AL4" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="N5" s="4">
+        <v>9898989899</v>
+      </c>
+      <c r="O5" s="4"/>
+      <c r="X5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="O6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>4444424444444440</v>
+      </c>
+      <c r="R6" s="5">
+        <v>8</v>
+      </c>
+      <c r="S6" s="3">
+        <v>2023</v>
+      </c>
+      <c r="T6">
+        <v>8</v>
+      </c>
+      <c r="U6" s="4">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
         <v>47</v>
       </c>
-      <c r="Y3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>33</v>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7">
+        <v>12345</v>
+      </c>
+      <c r="N7">
+        <v>9898989899</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="O4" t="s">
-        <v>37</v>
-      </c>
-      <c r="P4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>4444424444444440</v>
-      </c>
-      <c r="R4" s="5">
-        <v>8</v>
-      </c>
-      <c r="S4" s="3">
-        <v>2021</v>
-      </c>
-      <c r="T4">
-        <v>8</v>
-      </c>
-      <c r="U4" s="4">
-        <v>345</v>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8">
+        <v>12345</v>
+      </c>
+      <c r="N8">
+        <v>1211231311</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="9" spans="1:41" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD9" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE10" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5">
+      <c r="J12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12">
         <v>12345</v>
       </c>
-      <c r="N5">
-        <v>9898989899</v>
+      <c r="N12">
+        <v>1211231311</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN12" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO12" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Mahendra@123.com"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="Z3" r:id="rId3"/>
-    <hyperlink ref="AA3" r:id="rId4"/>
-    <hyperlink ref="H5" r:id="rId5"/>
-    <hyperlink ref="H2" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId1" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="Z5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="AA5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H8" r:id="rId7" xr:uid="{A911D6F8-BF05-4927-BAEE-D5D9E679A4A4}"/>
+    <hyperlink ref="H3" r:id="rId8" xr:uid="{8F34F70E-B126-4EB7-A65C-BE15598AB5F7}"/>
+    <hyperlink ref="H4" r:id="rId9" xr:uid="{934DC07D-98FD-4171-99F4-C545A13846FB}"/>
+    <hyperlink ref="B4" r:id="rId10" xr:uid="{52759A9F-3EB0-4ACF-BF56-E03D44C0BEBC}"/>
+    <hyperlink ref="H12" r:id="rId11" xr:uid="{4DA2C342-42C3-494E-AC2F-CA52CB370B94}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revlon Modular test cases & Hottools system test cases updates
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
+++ b/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B585D0AF-37C1-46BD-9F21-C804B5B899A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC5DCB0-4D96-4399-8497-2C7A4915B1ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="92">
   <si>
     <t>UserName</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Retailer_registration</t>
   </si>
   <si>
-    <t>harish.chiruvella1988@gmail.com</t>
-  </si>
-  <si>
     <t>Mini Travel Dryer in Mint</t>
   </si>
   <si>
@@ -273,7 +270,40 @@
     <t>Producttype</t>
   </si>
   <si>
-    <t>harish@test.com</t>
+    <t>stylist1711FF2@gmail.com</t>
+  </si>
+  <si>
+    <t>GiveUsFeedback</t>
+  </si>
+  <si>
+    <t>Hair Dryers</t>
+  </si>
+  <si>
+    <t>Nice Product. The Hair Dryers is a lightweight, compact tool with all the power of a full-sized dryer, adorned in a chic, amethyst hue.</t>
+  </si>
+  <si>
+    <t>ContactUs</t>
+  </si>
+  <si>
+    <t>DataCode</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Dryer</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Technical issues</t>
+  </si>
+  <si>
+    <t>retailer1911CC@gmail.com</t>
+  </si>
+  <si>
+    <t>stylist1911CC@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -647,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO12"/>
+  <dimension ref="A1:AR14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,9 +718,11 @@
     <col min="38" max="38" width="13.42578125" customWidth="1"/>
     <col min="39" max="39" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -785,37 +817,46 @@
         <v>57</v>
       </c>
       <c r="AF1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AK1" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="AL1" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AM1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="AN1" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="AO1" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -849,7 +890,7 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -867,17 +908,17 @@
         <v>49</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>44</v>
@@ -892,7 +933,7 @@
         <v>49</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
         <v>41</v>
@@ -915,16 +956,16 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AF4" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AG4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AH4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="AI4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AJ4">
         <v>30</v>
@@ -933,10 +974,10 @@
         <v>9898989899</v>
       </c>
       <c r="AL4" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:41" ht="60" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -946,7 +987,7 @@
       </c>
       <c r="O5" s="4"/>
       <c r="X5" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y5" t="s">
         <v>25</v>
@@ -961,7 +1002,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -988,7 +1029,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1023,7 +1064,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1058,7 +1099,7 @@
         <v>1211231311</v>
       </c>
     </row>
-    <row r="9" spans="1:41" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1072,7 +1113,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1080,20 +1121,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
         <v>61</v>
       </c>
-      <c r="C11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="H11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
         <v>45</v>
@@ -1126,10 +1170,71 @@
         <v>40</v>
       </c>
       <c r="AN12" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AO12" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14">
+        <v>12345</v>
+      </c>
+      <c r="N14">
+        <v>1211231311</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP14">
+        <v>1234</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1143,10 +1248,12 @@
     <hyperlink ref="H8" r:id="rId7" xr:uid="{A911D6F8-BF05-4927-BAEE-D5D9E679A4A4}"/>
     <hyperlink ref="H3" r:id="rId8" xr:uid="{8F34F70E-B126-4EB7-A65C-BE15598AB5F7}"/>
     <hyperlink ref="H4" r:id="rId9" xr:uid="{934DC07D-98FD-4171-99F4-C545A13846FB}"/>
-    <hyperlink ref="B4" r:id="rId10" xr:uid="{52759A9F-3EB0-4ACF-BF56-E03D44C0BEBC}"/>
-    <hyperlink ref="H12" r:id="rId11" xr:uid="{4DA2C342-42C3-494E-AC2F-CA52CB370B94}"/>
+    <hyperlink ref="H12" r:id="rId10" xr:uid="{4DA2C342-42C3-494E-AC2F-CA52CB370B94}"/>
+    <hyperlink ref="H11" r:id="rId11" xr:uid="{7BD4754A-594F-4961-AE0F-E1F56C66FD0B}"/>
+    <hyperlink ref="H13" r:id="rId12" xr:uid="{7A406351-FAB9-4E23-922B-489738F09821}"/>
+    <hyperlink ref="H14" r:id="rId13" xr:uid="{91142291-6DAE-469B-8AB3-1E0063EE5292}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mobile Execution Code changes for Revlon Us and Revlon UK NEw scripts and Helper.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
+++ b/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC5DCB0-4D96-4399-8497-2C7A4915B1ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5963C1A4-5F6C-45C7-A4F5-A90B9995FE0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hottools System Test cases Modified code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
+++ b/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5963C1A4-5F6C-45C7-A4F5-A90B9995FE0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C76E75A-69BD-424B-B3CB-291C6F5864C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="AX6" sqref="AX6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1132,7 @@
         <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
@@ -1249,9 +1249,9 @@
     <hyperlink ref="H3" r:id="rId8" xr:uid="{8F34F70E-B126-4EB7-A65C-BE15598AB5F7}"/>
     <hyperlink ref="H4" r:id="rId9" xr:uid="{934DC07D-98FD-4171-99F4-C545A13846FB}"/>
     <hyperlink ref="H12" r:id="rId10" xr:uid="{4DA2C342-42C3-494E-AC2F-CA52CB370B94}"/>
-    <hyperlink ref="H11" r:id="rId11" xr:uid="{7BD4754A-594F-4961-AE0F-E1F56C66FD0B}"/>
-    <hyperlink ref="H13" r:id="rId12" xr:uid="{7A406351-FAB9-4E23-922B-489738F09821}"/>
-    <hyperlink ref="H14" r:id="rId13" xr:uid="{91142291-6DAE-469B-8AB3-1E0063EE5292}"/>
+    <hyperlink ref="H13" r:id="rId11" xr:uid="{7A406351-FAB9-4E23-922B-489738F09821}"/>
+    <hyperlink ref="H14" r:id="rId12" xr:uid="{91142291-6DAE-469B-8AB3-1E0063EE5292}"/>
+    <hyperlink ref="H11" r:id="rId13" xr:uid="{6EA0AF11-6392-42EB-83B9-F15A1D4D2408}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>

</xml_diff>

<commit_message>
Hottools gold card,Distributor,stylist user,retailer user latest code changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
+++ b/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C76E75A-69BD-424B-B3CB-291C6F5864C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C9DA98-CCB1-4E12-B751-A60F794F5560}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="161">
   <si>
     <t>UserName</t>
   </si>
@@ -210,12 +202,6 @@
     <t>Mini Travel Dryer in Mint</t>
   </si>
   <si>
-    <t>alonsogarcia+pro@gmail.com</t>
-  </si>
-  <si>
-    <t>Testpro123</t>
-  </si>
-  <si>
     <t>DistributorAccountDetails</t>
   </si>
   <si>
@@ -304,6 +290,219 @@
   </si>
   <si>
     <t>stylist1911CC@gmail.com</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>01/26/2021</t>
+  </si>
+  <si>
+    <t>Guestshippingaddress</t>
+  </si>
+  <si>
+    <t>844 N Colony Rd</t>
+  </si>
+  <si>
+    <t>Wallingford</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>06492</t>
+  </si>
+  <si>
+    <t>Paypal</t>
+  </si>
+  <si>
+    <t>Skchinna28@gmail.com</t>
+  </si>
+  <si>
+    <t>Sravan@123</t>
+  </si>
+  <si>
+    <t>StylistCustomerAccountDetails</t>
+  </si>
+  <si>
+    <t>harish.chiruvella@gmail.com</t>
+  </si>
+  <si>
+    <t>ProdDistributorAccountDetails</t>
+  </si>
+  <si>
+    <t>testingPRO!@12</t>
+  </si>
+  <si>
+    <t>ezainos@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>devDistributorAccountDetails</t>
+  </si>
+  <si>
+    <t>kyle@321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  kyle321@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kyle321@gmail.com</t>
+  </si>
+  <si>
+    <t>PurchaseOrderDetails</t>
+  </si>
+  <si>
+    <t>OrderId</t>
+  </si>
+  <si>
+    <t>QuickOrderDetails</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>BecomeInfluencer</t>
+  </si>
+  <si>
+    <t>PersonalStyle</t>
+  </si>
+  <si>
+    <t>LikeProduct</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>InstaFollowers</t>
+  </si>
+  <si>
+    <t>Snapchat</t>
+  </si>
+  <si>
+    <t>snapFollower</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>FacebookFollowers</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TwitterFollowers</t>
+  </si>
+  <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>YoutubeFollowers</t>
+  </si>
+  <si>
+    <t>HeaderNames</t>
+  </si>
+  <si>
+    <t>Collections,One-Step Products,Curling Irons,Wands,Flat Irons,Hair Dryers,New!</t>
+  </si>
+  <si>
+    <t>HeaderLinks</t>
+  </si>
+  <si>
+    <t>HT1096BG</t>
+  </si>
+  <si>
+    <t>MultipleQuickOrderDetails</t>
+  </si>
+  <si>
+    <t>GoldCardDetails</t>
+  </si>
+  <si>
+    <t>InspoAccess</t>
+  </si>
+  <si>
+    <t>CreativeAccess</t>
+  </si>
+  <si>
+    <t>PT-JFPJH</t>
+  </si>
+  <si>
+    <t>WE-PLASF</t>
+  </si>
+  <si>
+    <t>ArtistAccess</t>
+  </si>
+  <si>
+    <t>PremiereAccess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH-ZYSWR </t>
+  </si>
+  <si>
+    <t>rmaddi@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Rakey0123@</t>
+  </si>
+  <si>
+    <t>AB-RHDCL</t>
+  </si>
+  <si>
+    <t>PromocodeproductName</t>
+  </si>
+  <si>
+    <t>Promocode</t>
+  </si>
+  <si>
+    <t>MODERN10</t>
+  </si>
+  <si>
+    <t>BLACK GOLD CURLING IRON 1-1/2"</t>
+  </si>
+  <si>
+    <t>AMEXCardDetails</t>
+  </si>
+  <si>
+    <t>MastercardDetails</t>
+  </si>
+  <si>
+    <t>DiscovercardDetails</t>
+  </si>
+  <si>
+    <t>AMEX</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>5500005555555559</t>
+  </si>
+  <si>
+    <t>Discover</t>
+  </si>
+  <si>
+    <t>6500000000000002</t>
+  </si>
+  <si>
+    <t>BLACK GOLD CURLING IRON 3/4"</t>
+  </si>
+  <si>
+    <t>HT1105BG,HT1096BG</t>
   </si>
 </sst>
 </file>
@@ -377,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -396,6 +595,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -677,10 +878,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR14"/>
+  <dimension ref="A1:BN29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,12 +899,13 @@
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.42578125" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17" customWidth="1"/>
+    <col min="20" max="20" width="11" customWidth="1"/>
     <col min="21" max="21" width="9.85546875" customWidth="1"/>
     <col min="22" max="22" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="69.42578125" customWidth="1"/>
     <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="24" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -720,9 +923,24 @@
     <col min="40" max="40" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="26.7109375" customWidth="1"/>
+    <col min="48" max="48" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -817,46 +1035,112 @@
         <v>57</v>
       </c>
       <c r="AF1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AJ1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="AL1" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AN1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AO1" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="AP1" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AQ1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AR1" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AS1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -890,7 +1174,7 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -908,17 +1192,17 @@
         <v>49</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>44</v>
@@ -933,7 +1217,7 @@
         <v>49</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I4" t="s">
         <v>41</v>
@@ -956,16 +1240,16 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AF4" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AG4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AH4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="AI4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AJ4">
         <v>30</v>
@@ -974,10 +1258,10 @@
         <v>9898989899</v>
       </c>
       <c r="AL4" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" ht="60" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:66" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -987,7 +1271,7 @@
       </c>
       <c r="O5" s="4"/>
       <c r="X5" s="9" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="Y5" t="s">
         <v>25</v>
@@ -1001,8 +1285,11 @@
       <c r="AD5" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AU5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1028,8 +1315,11 @@
       <c r="U6" s="4">
         <v>345</v>
       </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AT6">
+        <v>1234567890</v>
+      </c>
+    </row>
+    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1064,7 +1354,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1099,7 +1389,7 @@
         <v>1211231311</v>
       </c>
     </row>
-    <row r="9" spans="1:44" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1113,7 +1403,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1121,23 +1411,23 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
-        <v>61</v>
+      <c r="B11" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
         <v>45</v>
@@ -1158,7 +1448,7 @@
         <v>30</v>
       </c>
       <c r="L12" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="M12">
         <v>12345</v>
@@ -1166,19 +1456,28 @@
       <c r="N12">
         <v>1211231311</v>
       </c>
+      <c r="X12" t="s">
+        <v>59</v>
+      </c>
       <c r="AM12" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="AN12" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AO12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:44" ht="45" x14ac:dyDescent="0.25">
+      <c r="AP12">
+        <v>12345</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:66" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
         <v>45</v>
@@ -1187,15 +1486,15 @@
         <v>43</v>
       </c>
       <c r="X13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:66" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>82</v>
-      </c>
-      <c r="AD13" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:44" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>84</v>
       </c>
       <c r="D14" t="s">
         <v>45</v>
@@ -1225,16 +1524,350 @@
         <v>1211231311</v>
       </c>
       <c r="AD14" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AP14">
         <v>1234</v>
       </c>
       <c r="AQ14" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR14" t="s">
         <v>87</v>
       </c>
-      <c r="AR14" t="s">
-        <v>89</v>
+    </row>
+    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" t="s">
+        <v>96</v>
+      </c>
+      <c r="L15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="N15" s="4">
+        <v>9898989899</v>
+      </c>
+      <c r="O15" t="s">
+        <v>33</v>
+      </c>
+      <c r="P15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>4444424444444440</v>
+      </c>
+      <c r="R15">
+        <v>8</v>
+      </c>
+      <c r="S15" s="3">
+        <v>2023</v>
+      </c>
+      <c r="T15">
+        <v>8</v>
+      </c>
+      <c r="U15" s="4">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="AT20">
+        <v>1234567890</v>
+      </c>
+    </row>
+    <row r="21" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X21" t="s">
+        <v>134</v>
+      </c>
+      <c r="AU21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV22" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW22" t="s">
+        <v>126</v>
+      </c>
+      <c r="AX22" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY22" t="s">
+        <v>119</v>
+      </c>
+      <c r="AZ22">
+        <v>10</v>
+      </c>
+      <c r="BA22" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB22">
+        <v>10</v>
+      </c>
+      <c r="BC22" t="s">
+        <v>123</v>
+      </c>
+      <c r="BD22">
+        <v>10</v>
+      </c>
+      <c r="BE22" t="s">
+        <v>125</v>
+      </c>
+      <c r="BF22">
+        <v>10</v>
+      </c>
+      <c r="BG22" t="s">
+        <v>129</v>
+      </c>
+      <c r="BH22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>135</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X24" t="s">
+        <v>160</v>
+      </c>
+      <c r="AU24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" t="s">
+        <v>41</v>
+      </c>
+      <c r="J25" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" t="s">
+        <v>15</v>
+      </c>
+      <c r="M25">
+        <v>12345</v>
+      </c>
+      <c r="N25">
+        <v>9898989899</v>
+      </c>
+      <c r="BJ25" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK25" t="s">
+        <v>139</v>
+      </c>
+      <c r="BL25" t="s">
+        <v>140</v>
+      </c>
+      <c r="BM25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>147</v>
+      </c>
+      <c r="N26">
+        <v>9898989899</v>
+      </c>
+      <c r="X26" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BN26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>151</v>
+      </c>
+      <c r="P27" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>371449635398431</v>
+      </c>
+      <c r="R27">
+        <v>23</v>
+      </c>
+      <c r="S27">
+        <v>2023</v>
+      </c>
+      <c r="T27">
+        <v>8</v>
+      </c>
+      <c r="U27">
+        <v>3456</v>
+      </c>
+    </row>
+    <row r="28" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>152</v>
+      </c>
+      <c r="P28" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q28" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="R28">
+        <v>23</v>
+      </c>
+      <c r="S28">
+        <v>2023</v>
+      </c>
+      <c r="T28">
+        <v>8</v>
+      </c>
+      <c r="U28">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="29" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>153</v>
+      </c>
+      <c r="P29" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q29" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="R29">
+        <v>23</v>
+      </c>
+      <c r="S29">
+        <v>2023</v>
+      </c>
+      <c r="T29">
+        <v>8</v>
+      </c>
+      <c r="U29">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -1252,8 +1885,18 @@
     <hyperlink ref="H13" r:id="rId11" xr:uid="{7A406351-FAB9-4E23-922B-489738F09821}"/>
     <hyperlink ref="H14" r:id="rId12" xr:uid="{91142291-6DAE-469B-8AB3-1E0063EE5292}"/>
     <hyperlink ref="H11" r:id="rId13" xr:uid="{6EA0AF11-6392-42EB-83B9-F15A1D4D2408}"/>
+    <hyperlink ref="H15" r:id="rId14" xr:uid="{689684B6-DF24-400D-AB03-FDE92DCD608B}"/>
+    <hyperlink ref="B11" r:id="rId15" xr:uid="{022D5D14-D918-4A24-BE42-16123F687C0E}"/>
+    <hyperlink ref="C11" r:id="rId16" xr:uid="{AD354378-0168-4F47-AE81-EB6B14461BA9}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{1BD9CD3D-D594-4BE5-925D-2805D6E854D4}"/>
+    <hyperlink ref="H18" r:id="rId18" xr:uid="{702A798A-1E6D-4296-9B8D-A63D0F613281}"/>
+    <hyperlink ref="H21" r:id="rId19" xr:uid="{A7C939F8-463D-406B-8102-45677530F1F2}"/>
+    <hyperlink ref="H24" r:id="rId20" xr:uid="{99887349-959A-43BD-B8AE-275D77F78F51}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{9E4A78A6-3EE9-46B6-B0E6-2254587324BA}"/>
+    <hyperlink ref="Z26" r:id="rId22" xr:uid="{0DF84D34-530E-4B23-9430-10580E95F9E6}"/>
+    <hyperlink ref="AA26" r:id="rId23" xr:uid="{8B369FF0-D516-4AD3-994C-6510EC81782B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hottools latest code commit for stage environement changes of paypal and distributor logins
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
+++ b/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C9DA98-CCB1-4E12-B751-A60F794F5560}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22E7033-097A-465A-A1F8-0598DA350799}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="162">
   <si>
     <t>UserName</t>
   </si>
@@ -331,9 +331,6 @@
     <t>StylistCustomerAccountDetails</t>
   </si>
   <si>
-    <t>harish.chiruvella@gmail.com</t>
-  </si>
-  <si>
     <t>ProdDistributorAccountDetails</t>
   </si>
   <si>
@@ -454,12 +451,6 @@
     <t xml:space="preserve">TH-ZYSWR </t>
   </si>
   <si>
-    <t>rmaddi@helenoftroy.com</t>
-  </si>
-  <si>
-    <t>Rakey0123@</t>
-  </si>
-  <si>
     <t>AB-RHDCL</t>
   </si>
   <si>
@@ -503,6 +494,18 @@
   </si>
   <si>
     <t>HT1105BG,HT1096BG</t>
+  </si>
+  <si>
+    <t>vani.geetla12@gmail.com</t>
+  </si>
+  <si>
+    <t>Vihaan@2018</t>
+  </si>
+  <si>
+    <t>skasarla@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>geetlashravani1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -597,6 +600,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -880,9 +886,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BN29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W24" sqref="W24"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,78 +1083,78 @@
         <v>92</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AV1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AW1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="BE1" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="BF1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="BG1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="BI1" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="BJ1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="BK1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="BK1" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="BL1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BM1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="BM1" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="BN1" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>43</v>
+      <c r="B2" s="14" t="s">
+        <v>158</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
@@ -1160,7 +1166,7 @@
         <v>47</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="M2">
         <v>12345</v>
@@ -1271,7 +1277,7 @@
       </c>
       <c r="O5" s="4"/>
       <c r="X5" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Y5" t="s">
         <v>25</v>
@@ -1416,10 +1422,10 @@
         <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>89</v>
@@ -1605,44 +1611,44 @@
         <v>102</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" t="s">
-        <v>103</v>
+      <c r="C17" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="s">
         <v>107</v>
       </c>
-      <c r="B19" t="s">
+      <c r="H19" t="s">
         <v>109</v>
-      </c>
-      <c r="C19" t="s">
-        <v>108</v>
-      </c>
-      <c r="H19" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AT20">
         <v>1234567890</v>
@@ -1650,13 +1656,13 @@
     </row>
     <row r="21" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>43</v>
       </c>
       <c r="X21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AU21">
         <v>8</v>
@@ -1664,7 +1670,7 @@
     </row>
     <row r="22" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H22" t="s">
         <v>43</v>
@@ -1673,37 +1679,37 @@
         <v>85</v>
       </c>
       <c r="AW22" t="s">
+        <v>125</v>
+      </c>
+      <c r="AX22" t="s">
         <v>126</v>
       </c>
-      <c r="AX22" t="s">
-        <v>127</v>
-      </c>
       <c r="AY22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AZ22">
         <v>10</v>
       </c>
       <c r="BA22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="BB22">
         <v>10</v>
       </c>
       <c r="BC22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="BD22">
         <v>10</v>
       </c>
       <c r="BE22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BF22">
         <v>10</v>
       </c>
       <c r="BG22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="BH22">
         <v>10</v>
@@ -1711,21 +1717,21 @@
     </row>
     <row r="23" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="BI23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>43</v>
       </c>
       <c r="X24" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AU24">
         <v>6</v>
@@ -1733,7 +1739,7 @@
     </row>
     <row r="25" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>43</v>
@@ -1766,27 +1772,27 @@
         <v>9898989899</v>
       </c>
       <c r="BJ25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="BK25" t="s">
+        <v>138</v>
+      </c>
+      <c r="BL25" t="s">
         <v>139</v>
       </c>
-      <c r="BL25" t="s">
-        <v>140</v>
-      </c>
       <c r="BM25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="N26">
         <v>9898989899</v>
       </c>
       <c r="X26" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Y26" t="s">
         <v>25</v>
@@ -1798,15 +1804,15 @@
         <v>29</v>
       </c>
       <c r="BN26" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>148</v>
+      </c>
+      <c r="P27" t="s">
         <v>151</v>
-      </c>
-      <c r="P27" t="s">
-        <v>154</v>
       </c>
       <c r="Q27" s="3">
         <v>371449635398431</v>
@@ -1826,13 +1832,13 @@
     </row>
     <row r="28" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>149</v>
+      </c>
+      <c r="P28" t="s">
         <v>152</v>
       </c>
-      <c r="P28" t="s">
-        <v>155</v>
-      </c>
       <c r="Q28" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="R28">
         <v>23</v>
@@ -1849,13 +1855,13 @@
     </row>
     <row r="29" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="P29" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R29">
         <v>23</v>
@@ -1872,31 +1878,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="Z5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="AA5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H8" r:id="rId7" xr:uid="{A911D6F8-BF05-4927-BAEE-D5D9E679A4A4}"/>
-    <hyperlink ref="H3" r:id="rId8" xr:uid="{8F34F70E-B126-4EB7-A65C-BE15598AB5F7}"/>
-    <hyperlink ref="H4" r:id="rId9" xr:uid="{934DC07D-98FD-4171-99F4-C545A13846FB}"/>
-    <hyperlink ref="H12" r:id="rId10" xr:uid="{4DA2C342-42C3-494E-AC2F-CA52CB370B94}"/>
-    <hyperlink ref="H13" r:id="rId11" xr:uid="{7A406351-FAB9-4E23-922B-489738F09821}"/>
-    <hyperlink ref="H14" r:id="rId12" xr:uid="{91142291-6DAE-469B-8AB3-1E0063EE5292}"/>
-    <hyperlink ref="H11" r:id="rId13" xr:uid="{6EA0AF11-6392-42EB-83B9-F15A1D4D2408}"/>
-    <hyperlink ref="H15" r:id="rId14" xr:uid="{689684B6-DF24-400D-AB03-FDE92DCD608B}"/>
-    <hyperlink ref="B11" r:id="rId15" xr:uid="{022D5D14-D918-4A24-BE42-16123F687C0E}"/>
-    <hyperlink ref="C11" r:id="rId16" xr:uid="{AD354378-0168-4F47-AE81-EB6B14461BA9}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{1BD9CD3D-D594-4BE5-925D-2805D6E854D4}"/>
-    <hyperlink ref="H18" r:id="rId18" xr:uid="{702A798A-1E6D-4296-9B8D-A63D0F613281}"/>
-    <hyperlink ref="H21" r:id="rId19" xr:uid="{A7C939F8-463D-406B-8102-45677530F1F2}"/>
-    <hyperlink ref="H24" r:id="rId20" xr:uid="{99887349-959A-43BD-B8AE-275D77F78F51}"/>
-    <hyperlink ref="B25" r:id="rId21" xr:uid="{9E4A78A6-3EE9-46B6-B0E6-2254587324BA}"/>
-    <hyperlink ref="Z26" r:id="rId22" xr:uid="{0DF84D34-530E-4B23-9430-10580E95F9E6}"/>
-    <hyperlink ref="AA26" r:id="rId23" xr:uid="{8B369FF0-D516-4AD3-994C-6510EC81782B}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="Z5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="AA5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{A911D6F8-BF05-4927-BAEE-D5D9E679A4A4}"/>
+    <hyperlink ref="H3" r:id="rId7" xr:uid="{8F34F70E-B126-4EB7-A65C-BE15598AB5F7}"/>
+    <hyperlink ref="H4" r:id="rId8" xr:uid="{934DC07D-98FD-4171-99F4-C545A13846FB}"/>
+    <hyperlink ref="H12" r:id="rId9" xr:uid="{4DA2C342-42C3-494E-AC2F-CA52CB370B94}"/>
+    <hyperlink ref="H13" r:id="rId10" xr:uid="{7A406351-FAB9-4E23-922B-489738F09821}"/>
+    <hyperlink ref="H14" r:id="rId11" xr:uid="{91142291-6DAE-469B-8AB3-1E0063EE5292}"/>
+    <hyperlink ref="H11" r:id="rId12" xr:uid="{6EA0AF11-6392-42EB-83B9-F15A1D4D2408}"/>
+    <hyperlink ref="H15" r:id="rId13" xr:uid="{689684B6-DF24-400D-AB03-FDE92DCD608B}"/>
+    <hyperlink ref="B11" r:id="rId14" xr:uid="{022D5D14-D918-4A24-BE42-16123F687C0E}"/>
+    <hyperlink ref="C11" r:id="rId15" xr:uid="{AD354378-0168-4F47-AE81-EB6B14461BA9}"/>
+    <hyperlink ref="C18" r:id="rId16" xr:uid="{1BD9CD3D-D594-4BE5-925D-2805D6E854D4}"/>
+    <hyperlink ref="H18" r:id="rId17" xr:uid="{702A798A-1E6D-4296-9B8D-A63D0F613281}"/>
+    <hyperlink ref="H21" r:id="rId18" xr:uid="{A7C939F8-463D-406B-8102-45677530F1F2}"/>
+    <hyperlink ref="H24" r:id="rId19" xr:uid="{99887349-959A-43BD-B8AE-275D77F78F51}"/>
+    <hyperlink ref="B25" r:id="rId20" xr:uid="{9E4A78A6-3EE9-46B6-B0E6-2254587324BA}"/>
+    <hyperlink ref="Z26" r:id="rId21" xr:uid="{0DF84D34-530E-4B23-9430-10580E95F9E6}"/>
+    <hyperlink ref="AA26" r:id="rId22" xr:uid="{8B369FF0-D516-4AD3-994C-6510EC81782B}"/>
+    <hyperlink ref="B2" r:id="rId23" xr:uid="{EEC0292D-CAF3-4191-92EC-C2A797A35EFC}"/>
+    <hyperlink ref="H17" r:id="rId24" xr:uid="{BA90C0B7-86C2-4E69-9541-743AA5BBF479}"/>
+    <hyperlink ref="C17" r:id="rId25" xr:uid="{024B1394-A745-446B-A378-5981B002F328}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hottools 9 Expansion Test cases with Helper, TestData and testNG
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
+++ b/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22E7033-097A-465A-A1F8-0598DA350799}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E12957-090D-463B-B1B7-4BE710BABD75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="167">
   <si>
     <t>UserName</t>
   </si>
@@ -460,9 +460,6 @@
     <t>Promocode</t>
   </si>
   <si>
-    <t>MODERN10</t>
-  </si>
-  <si>
     <t>BLACK GOLD CURLING IRON 1-1/2"</t>
   </si>
   <si>
@@ -506,6 +503,24 @@
   </si>
   <si>
     <t>geetlashravani1@gmail.com</t>
+  </si>
+  <si>
+    <t>QAPROMO15</t>
+  </si>
+  <si>
+    <t>DistributorPromocode</t>
+  </si>
+  <si>
+    <t>StylistPromocode</t>
+  </si>
+  <si>
+    <t>QAPROMO10</t>
+  </si>
+  <si>
+    <t>SHOPHT5</t>
+  </si>
+  <si>
+    <t>License Expiration Date1</t>
   </si>
 </sst>
 </file>
@@ -884,11 +899,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BN29"/>
+  <dimension ref="A1:BO31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BO1" sqref="BO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,9 +959,11 @@
     <col min="64" max="64" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="19.140625" customWidth="1"/>
+    <col min="67" max="67" width="23" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1145,16 +1162,19 @@
       <c r="BN1" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BO1" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
@@ -1166,7 +1186,7 @@
         <v>47</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M2">
         <v>12345</v>
@@ -1180,7 +1200,7 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1203,7 +1223,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1266,8 +1286,11 @@
       <c r="AL4" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" spans="1:66" ht="60" x14ac:dyDescent="0.25">
+      <c r="BO4" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:67" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1277,7 +1300,7 @@
       </c>
       <c r="O5" s="4"/>
       <c r="X5" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Y5" t="s">
         <v>25</v>
@@ -1295,7 +1318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1325,7 +1348,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1360,7 +1383,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1395,7 +1418,7 @@
         <v>1211231311</v>
       </c>
     </row>
-    <row r="9" spans="1:66" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1409,7 +1432,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1417,21 +1440,21 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -1481,7 +1504,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:66" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:67" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -1498,7 +1521,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:66" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:67" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -1542,7 +1565,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -1595,7 +1618,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -1612,10 +1635,10 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:66" x14ac:dyDescent="0.25">
@@ -1731,7 +1754,7 @@
         <v>43</v>
       </c>
       <c r="X24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AU24">
         <v>6</v>
@@ -1792,7 +1815,7 @@
         <v>9898989899</v>
       </c>
       <c r="X26" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Y26" t="s">
         <v>25</v>
@@ -1804,15 +1827,15 @@
         <v>29</v>
       </c>
       <c r="BN26" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q27" s="3">
         <v>371449635398431</v>
@@ -1832,13 +1855,13 @@
     </row>
     <row r="28" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P28" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q28" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="Q28" s="13" t="s">
-        <v>153</v>
       </c>
       <c r="R28">
         <v>23</v>
@@ -1855,13 +1878,13 @@
     </row>
     <row r="29" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P29" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q29" s="13" t="s">
         <v>154</v>
-      </c>
-      <c r="Q29" s="13" t="s">
-        <v>155</v>
       </c>
       <c r="R29">
         <v>23</v>
@@ -1874,6 +1897,22 @@
       </c>
       <c r="U29">
         <v>345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>162</v>
+      </c>
+      <c r="BN30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>163</v>
+      </c>
+      <c r="BN31" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I have updated Hottools code.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
+++ b/src/test/resources/TestData/Hottools/HottoolsTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E12957-090D-463B-B1B7-4BE710BABD75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A801E893-5B66-4D37-8A62-4B3FD49D736E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="177">
   <si>
     <t>UserName</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Company</t>
   </si>
   <si>
-    <t>Louteswave</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -151,21 +148,6 @@
     <t>HOT TOOLS AMETHYST DRYER</t>
   </si>
   <si>
-    <t>harish.chiruvella1@gmail.com</t>
-  </si>
-  <si>
-    <t>Harish!123</t>
-  </si>
-  <si>
-    <t>Harish</t>
-  </si>
-  <si>
-    <t>Chiruvella</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Addressbook</t>
   </si>
   <si>
@@ -256,9 +238,6 @@
     <t>Producttype</t>
   </si>
   <si>
-    <t>stylist1711FF2@gmail.com</t>
-  </si>
-  <si>
     <t>GiveUsFeedback</t>
   </si>
   <si>
@@ -286,12 +265,6 @@
     <t>Technical issues</t>
   </si>
   <si>
-    <t>retailer1911CC@gmail.com</t>
-  </si>
-  <si>
-    <t>stylist1911CC@gmail.com</t>
-  </si>
-  <si>
     <t>CA</t>
   </si>
   <si>
@@ -421,9 +394,6 @@
     <t>HeaderLinks</t>
   </si>
   <si>
-    <t>HT1096BG</t>
-  </si>
-  <si>
     <t>MultipleQuickOrderDetails</t>
   </si>
   <si>
@@ -490,12 +460,6 @@
     <t>BLACK GOLD CURLING IRON 3/4"</t>
   </si>
   <si>
-    <t>HT1105BG,HT1096BG</t>
-  </si>
-  <si>
-    <t>vani.geetla12@gmail.com</t>
-  </si>
-  <si>
     <t>Vihaan@2018</t>
   </si>
   <si>
@@ -505,9 +469,6 @@
     <t>geetlashravani1@gmail.com</t>
   </si>
   <si>
-    <t>QAPROMO15</t>
-  </si>
-  <si>
     <t>DistributorPromocode</t>
   </si>
   <si>
@@ -521,6 +482,75 @@
   </si>
   <si>
     <t>License Expiration Date1</t>
+  </si>
+  <si>
+    <t>dtc.qatesting.hottools@gmail.com</t>
+  </si>
+  <si>
+    <t>Lotuswave123</t>
+  </si>
+  <si>
+    <t>dtc.qatesting1.hottools@gmail.com</t>
+  </si>
+  <si>
+    <t>Skasarla@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>0123456789</t>
+  </si>
+  <si>
+    <t>RK</t>
+  </si>
+  <si>
+    <t>rajkumar</t>
+  </si>
+  <si>
+    <t>HT1101BG</t>
+  </si>
+  <si>
+    <t>HT1101BG GH9207</t>
+  </si>
+  <si>
+    <t>PoBoxAddress</t>
+  </si>
+  <si>
+    <t>QATesting</t>
+  </si>
+  <si>
+    <t>Hottools</t>
+  </si>
+  <si>
+    <t>Flagstaff</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Po Box 9998, Flagstaff, Arizona, 86011</t>
+  </si>
+  <si>
+    <t>Differentbillingaddress</t>
+  </si>
+  <si>
+    <t>QA Testing</t>
+  </si>
+  <si>
+    <t>Newark</t>
+  </si>
+  <si>
+    <t>715 Christiana Mall</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>No_tax_address</t>
+  </si>
+  <si>
+    <t>TEST10OFF</t>
+  </si>
+  <si>
+    <t>EmployeeAccountDetails</t>
   </si>
 </sst>
 </file>
@@ -594,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -618,6 +648,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -899,25 +930,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BO31"/>
+  <dimension ref="A1:BO35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BO1" sqref="BO1"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AU23" sqref="AU23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" customWidth="1"/>
     <col min="9" max="9" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.42578125" customWidth="1"/>
     <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -992,7 +1024,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>7</v>
@@ -1046,124 +1078,124 @@
         <v>28</v>
       </c>
       <c r="AB1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AF1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AF1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="AH1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL1" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN1" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AQ1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="AT1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="BA1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="BC1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="BE1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AW1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="BC1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="BE1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="BK1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="BG1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BH1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="BJ1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="BK1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BL1" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="BM1" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="BN1" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="BO1" s="2" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.25">
@@ -1171,22 +1203,22 @@
         <v>34</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>159</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>165</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M2">
         <v>12345</v>
@@ -1202,54 +1234,54 @@
     </row>
     <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>155</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>78</v>
+        <v>156</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>89</v>
+        <v>156</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" t="s">
         <v>30</v>
@@ -1266,16 +1298,16 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AF4" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="AG4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="AH4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="AI4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="AJ4">
         <v>30</v>
@@ -1284,10 +1316,10 @@
         <v>9898989899</v>
       </c>
       <c r="AL4" s="10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="BO4" s="12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:67" ht="60" x14ac:dyDescent="0.25">
@@ -1295,12 +1327,21 @@
         <v>22</v>
       </c>
       <c r="C5" s="1"/>
+      <c r="D5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
       <c r="N5" s="4">
         <v>9898989899</v>
       </c>
       <c r="O5" s="4"/>
       <c r="X5" s="9" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="Y5" t="s">
         <v>25</v>
@@ -1312,7 +1353,7 @@
         <v>29</v>
       </c>
       <c r="AD5" s="6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AU5">
         <v>17</v>
@@ -1323,6 +1364,15 @@
         <v>18</v>
       </c>
       <c r="C6" s="1"/>
+      <c r="D6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
       <c r="O6" t="s">
         <v>33</v>
       </c>
@@ -1344,66 +1394,75 @@
       <c r="U6" s="4">
         <v>345</v>
       </c>
-      <c r="AT6">
-        <v>1234567890</v>
+      <c r="AT6" s="12" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>165</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>172</v>
       </c>
       <c r="J7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>30</v>
+        <v>171</v>
       </c>
       <c r="L7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="M7">
-        <v>12345</v>
+        <v>19702</v>
       </c>
       <c r="N7">
         <v>9898989899</v>
       </c>
+      <c r="O7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="3"/>
+      <c r="U7" s="4"/>
+      <c r="AT7" s="12"/>
     </row>
     <row r="8" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>165</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>156</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K8" t="s">
         <v>30</v>
@@ -1415,136 +1474,139 @@
         <v>12345</v>
       </c>
       <c r="N8">
-        <v>1211231311</v>
-      </c>
-    </row>
-    <row r="9" spans="1:67" ht="60" x14ac:dyDescent="0.25">
+        <v>9898989899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD9" s="6" t="s">
-        <v>54</v>
+        <v>169</v>
+      </c>
+      <c r="D9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE10" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" t="s">
+        <v>165</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10">
+        <v>12345</v>
+      </c>
+      <c r="N10">
+        <v>1211231311</v>
+      </c>
+    </row>
+    <row r="11" spans="1:67" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>89</v>
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>170</v>
+      </c>
+      <c r="F11" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD11" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" t="s">
+        <v>165</v>
+      </c>
+      <c r="AE12" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" t="s">
+        <v>165</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" t="s">
+        <v>165</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I14" t="s">
         <v>40</v>
       </c>
-      <c r="K12" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" t="s">
-        <v>90</v>
-      </c>
-      <c r="M12">
-        <v>12345</v>
-      </c>
-      <c r="N12">
-        <v>1211231311</v>
-      </c>
-      <c r="X12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM12" t="s">
-        <v>91</v>
-      </c>
-      <c r="AN12" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP12">
-        <v>12345</v>
-      </c>
-      <c r="AS12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:67" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="X13" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD13" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:67" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I14" t="s">
-        <v>41</v>
-      </c>
       <c r="J14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K14" t="s">
         <v>30</v>
       </c>
       <c r="L14" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="M14">
         <v>12345</v>
@@ -1552,339 +1614,423 @@
       <c r="N14">
         <v>1211231311</v>
       </c>
-      <c r="AD14" s="6" t="s">
-        <v>81</v>
+      <c r="X14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN14" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>53</v>
       </c>
       <c r="AP14">
+        <v>12345</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:67" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X15" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD15" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:67" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" t="s">
+        <v>170</v>
+      </c>
+      <c r="F16" t="s">
+        <v>165</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16">
+        <v>12345</v>
+      </c>
+      <c r="N16">
+        <v>1211231311</v>
+      </c>
+      <c r="AD16" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP16">
         <v>1234</v>
       </c>
-      <c r="AQ14" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" t="s">
-        <v>95</v>
-      </c>
-      <c r="J15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" t="s">
-        <v>96</v>
-      </c>
-      <c r="L15" t="s">
-        <v>97</v>
-      </c>
-      <c r="M15" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="N15" s="4">
-        <v>9898989899</v>
-      </c>
-      <c r="O15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P15" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>4444424444444440</v>
-      </c>
-      <c r="R15">
-        <v>8</v>
-      </c>
-      <c r="S15" s="3">
-        <v>2023</v>
-      </c>
-      <c r="T15">
-        <v>8</v>
-      </c>
-      <c r="U15" s="4">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" t="s">
-        <v>101</v>
+      <c r="AQ16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
-        <v>158</v>
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F17" t="s">
+        <v>165</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
+      </c>
+      <c r="I17" t="s">
+        <v>86</v>
+      </c>
+      <c r="J17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L17" t="s">
+        <v>88</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="N17" s="4">
+        <v>9898989899</v>
+      </c>
+      <c r="O17" t="s">
+        <v>33</v>
+      </c>
+      <c r="P17" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>4444424444444440</v>
+      </c>
+      <c r="R17">
+        <v>8</v>
+      </c>
+      <c r="S17" s="3">
+        <v>2023</v>
+      </c>
+      <c r="T17">
+        <v>8</v>
+      </c>
+      <c r="U17" s="4">
+        <v>345</v>
       </c>
     </row>
     <row r="18" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>105</v>
+        <v>92</v>
+      </c>
+      <c r="D18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F18" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" t="s">
-        <v>109</v>
+        <v>93</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D19" t="s">
+        <v>170</v>
+      </c>
+      <c r="F19" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>110</v>
-      </c>
-      <c r="AT20">
-        <v>1234567890</v>
+        <v>94</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>112</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="X21" t="s">
-        <v>133</v>
-      </c>
-      <c r="AU21">
-        <v>8</v>
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>170</v>
+      </c>
+      <c r="F21" t="s">
+        <v>165</v>
+      </c>
+      <c r="H21" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>114</v>
-      </c>
-      <c r="H22" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV22" t="s">
-        <v>85</v>
-      </c>
-      <c r="AW22" t="s">
-        <v>125</v>
-      </c>
-      <c r="AX22" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY22" t="s">
-        <v>118</v>
-      </c>
-      <c r="AZ22">
-        <v>10</v>
-      </c>
-      <c r="BA22" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB22">
-        <v>10</v>
-      </c>
-      <c r="BC22" t="s">
-        <v>122</v>
-      </c>
-      <c r="BD22">
-        <v>10</v>
-      </c>
-      <c r="BE22" t="s">
-        <v>124</v>
-      </c>
-      <c r="BF22">
-        <v>10</v>
-      </c>
-      <c r="BG22" t="s">
-        <v>128</v>
-      </c>
-      <c r="BH22">
-        <v>10</v>
+        <v>101</v>
+      </c>
+      <c r="D22" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" t="s">
+        <v>165</v>
+      </c>
+      <c r="AT22">
+        <v>1234567890</v>
       </c>
     </row>
     <row r="23" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>132</v>
-      </c>
-      <c r="BI23" t="s">
-        <v>131</v>
+        <v>103</v>
+      </c>
+      <c r="D23" t="s">
+        <v>170</v>
+      </c>
+      <c r="F23" t="s">
+        <v>165</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X23" t="s">
+        <v>161</v>
+      </c>
+      <c r="AU23">
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>134</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="X24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" t="s">
+        <v>170</v>
+      </c>
+      <c r="F24" t="s">
+        <v>165</v>
+      </c>
+      <c r="H24" t="s">
         <v>156</v>
       </c>
-      <c r="AU24">
-        <v>6</v>
+      <c r="AV24" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AX24" t="s">
+        <v>117</v>
+      </c>
+      <c r="AY24" t="s">
+        <v>109</v>
+      </c>
+      <c r="AZ24">
+        <v>10</v>
+      </c>
+      <c r="BA24" t="s">
+        <v>111</v>
+      </c>
+      <c r="BB24">
+        <v>10</v>
+      </c>
+      <c r="BC24" t="s">
+        <v>113</v>
+      </c>
+      <c r="BD24">
+        <v>10</v>
+      </c>
+      <c r="BE24" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF24">
+        <v>10</v>
+      </c>
+      <c r="BG24" t="s">
+        <v>119</v>
+      </c>
+      <c r="BH24">
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>43</v>
+        <v>123</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
       <c r="F25" t="s">
-        <v>46</v>
-      </c>
-      <c r="H25" t="s">
-        <v>43</v>
-      </c>
-      <c r="I25" t="s">
-        <v>41</v>
-      </c>
-      <c r="J25" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" t="s">
-        <v>30</v>
-      </c>
-      <c r="L25" t="s">
-        <v>15</v>
-      </c>
-      <c r="M25">
-        <v>12345</v>
-      </c>
-      <c r="N25">
-        <v>9898989899</v>
-      </c>
-      <c r="BJ25" t="s">
-        <v>143</v>
-      </c>
-      <c r="BK25" t="s">
-        <v>138</v>
-      </c>
-      <c r="BL25" t="s">
-        <v>139</v>
-      </c>
-      <c r="BM25" t="s">
-        <v>142</v>
+        <v>165</v>
+      </c>
+      <c r="BI25" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>144</v>
-      </c>
-      <c r="N26">
-        <v>9898989899</v>
-      </c>
-      <c r="X26" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="BN26" t="s">
-        <v>161</v>
+        <v>124</v>
+      </c>
+      <c r="D26" t="s">
+        <v>170</v>
+      </c>
+      <c r="F26" t="s">
+        <v>165</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X26" t="s">
+        <v>162</v>
+      </c>
+      <c r="AU26">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>147</v>
-      </c>
-      <c r="P27" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q27" s="3">
-        <v>371449635398431</v>
-      </c>
-      <c r="R27">
-        <v>23</v>
-      </c>
-      <c r="S27">
-        <v>2023</v>
-      </c>
-      <c r="T27">
-        <v>8</v>
-      </c>
-      <c r="U27">
-        <v>3456</v>
+        <v>125</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" t="s">
+        <v>170</v>
+      </c>
+      <c r="F27" t="s">
+        <v>165</v>
+      </c>
+      <c r="H27" t="s">
+        <v>156</v>
+      </c>
+      <c r="I27" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" t="s">
+        <v>30</v>
+      </c>
+      <c r="L27" t="s">
+        <v>15</v>
+      </c>
+      <c r="M27">
+        <v>12345</v>
+      </c>
+      <c r="N27">
+        <v>9898989899</v>
+      </c>
+      <c r="BJ27" t="s">
+        <v>133</v>
+      </c>
+      <c r="BK27" t="s">
+        <v>128</v>
+      </c>
+      <c r="BL27" t="s">
+        <v>129</v>
+      </c>
+      <c r="BM27" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>148</v>
-      </c>
-      <c r="P28" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q28" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="R28">
-        <v>23</v>
-      </c>
-      <c r="S28">
-        <v>2023</v>
-      </c>
-      <c r="T28">
-        <v>8</v>
-      </c>
-      <c r="U28">
-        <v>345</v>
+        <v>134</v>
+      </c>
+      <c r="F28" t="s">
+        <v>165</v>
+      </c>
+      <c r="N28">
+        <v>9898989899</v>
+      </c>
+      <c r="X28" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BN28" s="15" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>137</v>
+      </c>
+      <c r="F29" t="s">
+        <v>165</v>
       </c>
       <c r="P29" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q29" s="13" t="s">
-        <v>154</v>
+        <v>140</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>371449635398431</v>
       </c>
       <c r="R29">
         <v>23</v>
@@ -1896,54 +2042,184 @@
         <v>8</v>
       </c>
       <c r="U29">
-        <v>345</v>
+        <v>3456</v>
       </c>
     </row>
     <row r="30" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>162</v>
-      </c>
-      <c r="BN30" t="s">
-        <v>164</v>
+        <v>138</v>
+      </c>
+      <c r="F30" t="s">
+        <v>165</v>
+      </c>
+      <c r="P30" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q30" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="R30">
+        <v>23</v>
+      </c>
+      <c r="S30">
+        <v>2023</v>
+      </c>
+      <c r="T30">
+        <v>8</v>
+      </c>
+      <c r="U30">
+        <v>345</v>
       </c>
     </row>
     <row r="31" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31" t="s">
+        <v>165</v>
+      </c>
+      <c r="P31" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q31" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="R31">
+        <v>23</v>
+      </c>
+      <c r="S31">
+        <v>2023</v>
+      </c>
+      <c r="T31">
+        <v>8</v>
+      </c>
+      <c r="U31">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="32" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>149</v>
+      </c>
+      <c r="F32" t="s">
+        <v>165</v>
+      </c>
+      <c r="AT32" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="BN32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="F33" t="s">
+        <v>165</v>
+      </c>
+      <c r="BN33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:66" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>163</v>
       </c>
-      <c r="BN31" t="s">
-        <v>165</v>
-      </c>
+      <c r="D34" t="s">
+        <v>164</v>
+      </c>
+      <c r="F34" t="s">
+        <v>165</v>
+      </c>
+      <c r="G34" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="I34" t="s">
+        <v>168</v>
+      </c>
+      <c r="J34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K34" t="s">
+        <v>166</v>
+      </c>
+      <c r="L34" t="s">
+        <v>167</v>
+      </c>
+      <c r="M34">
+        <v>86011</v>
+      </c>
+      <c r="N34">
+        <v>8798545632</v>
+      </c>
+    </row>
+    <row r="35" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>176</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" t="s">
+        <v>165</v>
+      </c>
+      <c r="G35" t="s">
+        <v>43</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId1" display="Vihaan@2018" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="Z5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="AA5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="H7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{A911D6F8-BF05-4927-BAEE-D5D9E679A4A4}"/>
+    <hyperlink ref="H8" r:id="rId5" display="harish.chiruvella1@gmail.com" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H10" r:id="rId6" display="harish.chiruvella1@gmail.com" xr:uid="{A911D6F8-BF05-4927-BAEE-D5D9E679A4A4}"/>
     <hyperlink ref="H3" r:id="rId7" xr:uid="{8F34F70E-B126-4EB7-A65C-BE15598AB5F7}"/>
     <hyperlink ref="H4" r:id="rId8" xr:uid="{934DC07D-98FD-4171-99F4-C545A13846FB}"/>
-    <hyperlink ref="H12" r:id="rId9" xr:uid="{4DA2C342-42C3-494E-AC2F-CA52CB370B94}"/>
-    <hyperlink ref="H13" r:id="rId10" xr:uid="{7A406351-FAB9-4E23-922B-489738F09821}"/>
-    <hyperlink ref="H14" r:id="rId11" xr:uid="{91142291-6DAE-469B-8AB3-1E0063EE5292}"/>
-    <hyperlink ref="H11" r:id="rId12" xr:uid="{6EA0AF11-6392-42EB-83B9-F15A1D4D2408}"/>
-    <hyperlink ref="H15" r:id="rId13" xr:uid="{689684B6-DF24-400D-AB03-FDE92DCD608B}"/>
-    <hyperlink ref="B11" r:id="rId14" xr:uid="{022D5D14-D918-4A24-BE42-16123F687C0E}"/>
-    <hyperlink ref="C11" r:id="rId15" xr:uid="{AD354378-0168-4F47-AE81-EB6B14461BA9}"/>
-    <hyperlink ref="C18" r:id="rId16" xr:uid="{1BD9CD3D-D594-4BE5-925D-2805D6E854D4}"/>
-    <hyperlink ref="H18" r:id="rId17" xr:uid="{702A798A-1E6D-4296-9B8D-A63D0F613281}"/>
-    <hyperlink ref="H21" r:id="rId18" xr:uid="{A7C939F8-463D-406B-8102-45677530F1F2}"/>
-    <hyperlink ref="H24" r:id="rId19" xr:uid="{99887349-959A-43BD-B8AE-275D77F78F51}"/>
-    <hyperlink ref="B25" r:id="rId20" xr:uid="{9E4A78A6-3EE9-46B6-B0E6-2254587324BA}"/>
-    <hyperlink ref="Z26" r:id="rId21" xr:uid="{0DF84D34-530E-4B23-9430-10580E95F9E6}"/>
-    <hyperlink ref="AA26" r:id="rId22" xr:uid="{8B369FF0-D516-4AD3-994C-6510EC81782B}"/>
+    <hyperlink ref="H14" r:id="rId9" display="harish.chiruvella1@gmail.com" xr:uid="{4DA2C342-42C3-494E-AC2F-CA52CB370B94}"/>
+    <hyperlink ref="H15" r:id="rId10" display="harish.chiruvella1@gmail.com" xr:uid="{7A406351-FAB9-4E23-922B-489738F09821}"/>
+    <hyperlink ref="H16" r:id="rId11" display="harish.chiruvella1@gmail.com" xr:uid="{91142291-6DAE-469B-8AB3-1E0063EE5292}"/>
+    <hyperlink ref="H13" r:id="rId12" xr:uid="{6EA0AF11-6392-42EB-83B9-F15A1D4D2408}"/>
+    <hyperlink ref="H17" r:id="rId13" display="harish.chiruvella1@gmail.com" xr:uid="{689684B6-DF24-400D-AB03-FDE92DCD608B}"/>
+    <hyperlink ref="B13" r:id="rId14" xr:uid="{022D5D14-D918-4A24-BE42-16123F687C0E}"/>
+    <hyperlink ref="C13" r:id="rId15" xr:uid="{AD354378-0168-4F47-AE81-EB6B14461BA9}"/>
+    <hyperlink ref="C20" r:id="rId16" xr:uid="{1BD9CD3D-D594-4BE5-925D-2805D6E854D4}"/>
+    <hyperlink ref="H20" r:id="rId17" xr:uid="{702A798A-1E6D-4296-9B8D-A63D0F613281}"/>
+    <hyperlink ref="H23" r:id="rId18" display="harish.chiruvella1@gmail.com" xr:uid="{A7C939F8-463D-406B-8102-45677530F1F2}"/>
+    <hyperlink ref="H26" r:id="rId19" display="harish.chiruvella1@gmail.com" xr:uid="{99887349-959A-43BD-B8AE-275D77F78F51}"/>
+    <hyperlink ref="B27" r:id="rId20" display="harish.chiruvella1@gmail.com" xr:uid="{9E4A78A6-3EE9-46B6-B0E6-2254587324BA}"/>
+    <hyperlink ref="Z28" r:id="rId21" xr:uid="{0DF84D34-530E-4B23-9430-10580E95F9E6}"/>
+    <hyperlink ref="AA28" r:id="rId22" xr:uid="{8B369FF0-D516-4AD3-994C-6510EC81782B}"/>
     <hyperlink ref="B2" r:id="rId23" xr:uid="{EEC0292D-CAF3-4191-92EC-C2A797A35EFC}"/>
-    <hyperlink ref="H17" r:id="rId24" xr:uid="{BA90C0B7-86C2-4E69-9541-743AA5BBF479}"/>
-    <hyperlink ref="C17" r:id="rId25" xr:uid="{024B1394-A745-446B-A378-5981B002F328}"/>
+    <hyperlink ref="H19" r:id="rId24" xr:uid="{BA90C0B7-86C2-4E69-9541-743AA5BBF479}"/>
+    <hyperlink ref="C19" r:id="rId25" xr:uid="{024B1394-A745-446B-A378-5981B002F328}"/>
+    <hyperlink ref="B4" r:id="rId26" xr:uid="{69D07A28-3DEE-45A0-A546-3962C2E7DFBF}"/>
+    <hyperlink ref="B18" r:id="rId27" xr:uid="{01641F53-C1C4-434D-AA97-F48BFE0D5CC5}"/>
+    <hyperlink ref="C18" r:id="rId28" xr:uid="{2CCE0133-9532-46EA-9F98-55BCE758A193}"/>
+    <hyperlink ref="H34" r:id="rId29" xr:uid="{293F07C9-18C9-4367-9737-510F75A02958}"/>
+    <hyperlink ref="H9" r:id="rId30" display="harish.chiruvella1@gmail.com" xr:uid="{6D91902C-D274-43D8-92A5-CD6CED655B7B}"/>
+    <hyperlink ref="H7" r:id="rId31" display="harish.chiruvella1@gmail.com" xr:uid="{37C44DF0-CED3-46ED-9B92-133CC733D381}"/>
+    <hyperlink ref="B35" r:id="rId32" xr:uid="{6285E773-965A-47A9-B10E-7F18938CE69F}"/>
+    <hyperlink ref="C35" r:id="rId33" xr:uid="{842F33BC-F318-40EE-8A33-5FAE596265AD}"/>
+    <hyperlink ref="H35" r:id="rId34" xr:uid="{543563EB-B538-4FC6-ACC7-696DD588894F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId26"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>